<commit_message>
FOUND ERROR IN LAB PART 3
</commit_message>
<xml_diff>
--- a/experiment3data1.xlsx
+++ b/experiment3data1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mallen/Documents/128AL/JohnsonNoise128AL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CD667CD-AF92-5D44-A334-4A078400E705}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698134FB-8EF8-6247-9679-3DCFACF3BBAC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="460" windowWidth="27240" windowHeight="16440" xr2:uid="{36B4CA7B-A577-6142-878E-A287F2DD9FD6}"/>
+    <workbookView xWindow="6360" yWindow="460" windowWidth="27240" windowHeight="16440" xr2:uid="{36B4CA7B-A577-6142-878E-A287F2DD9FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,19 +494,19 @@
         <v>4.7679999999999998E-5</v>
       </c>
       <c r="F2" s="1">
-        <v>4.7919999999999999E-4</v>
+        <v>4.7920000000000002E-5</v>
       </c>
       <c r="G2">
         <f>AVERAGE(B2:F2)</f>
-        <v>1.3399200000000001E-4</v>
+        <v>4.7736000000000005E-5</v>
       </c>
       <c r="H2">
         <f>STDEV(B2:G2)</f>
-        <v>1.7260404658060597E-4</v>
+        <v>1.566652482205289E-7</v>
       </c>
       <c r="I2">
         <f>H2/SQRT(5)</f>
-        <v>7.7190876269155013E-5</v>
+        <v>7.0062828946596106E-8</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>